<commit_message>
Added jump sound effect and tried to add background music, but it won't loop!?
</commit_message>
<xml_diff>
--- a/assets/segments/segment_plans.xlsx
+++ b/assets/segments/segment_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Flutter\cookie_monster\assets\segments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A862322-4DAB-4987-9DD8-97D19D4FB7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F89BC80-DFE5-4D33-B57D-A657C2F532D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{5D161934-754C-46FF-97FA-09F80D988C11}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{5D161934-754C-46FF-97FA-09F80D988C11}"/>
   </bookViews>
   <sheets>
     <sheet name="Segment0" sheetId="1" r:id="rId1"/>
@@ -1185,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57244EC7-BEC6-45A9-BA50-DF8EFBBE0C7C}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1810,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5645CD27-838A-43A2-A6C6-350E89854574}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>